<commit_message>
test scripts Home, Find pages
</commit_message>
<xml_diff>
--- a/Assignment_TestCases.xlsx
+++ b/Assignment_TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/Documents/Working/Personal/assignment-vdc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1CDAEDB-517F-7E4B-833F-4A046A6E7243}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9FD7CBB-A5F4-DD48-968A-0076324B4888}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="980" yWindow="500" windowWidth="27820" windowHeight="17500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="980" yWindow="500" windowWidth="27820" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General report" sheetId="8" r:id="rId1"/>
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="199">
   <si>
     <t>Steps</t>
   </si>
@@ -325,9 +325,6 @@
   </si>
   <si>
     <t>Medium</t>
-  </si>
-  <si>
-    <t>Test Case 7: Input invalid city like maximum characters in the "Weather in you city" search box and select Enter on the keyboard</t>
   </si>
   <si>
     <t>Input maximum characters of the search box
@@ -1326,6 +1323,15 @@
       </rPr>
       <t xml:space="preserve"> Please refer to the attached file JSON</t>
     </r>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Test Case 7: Input invalid city like 100 characters in the "Weather in you city" search box and select Enter on the keyboard</t>
   </si>
 </sst>
 </file>
@@ -1972,7 +1978,75 @@
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="153">
+  <dxfs count="159">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE79B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE79B"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -6251,9 +6325,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K35" sqref="K35:K38"/>
+    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="2" ySplit="4" topLeftCell="C21" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="G40" sqref="G40:G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6295,7 +6371,7 @@
       <c r="A2" s="45"/>
       <c r="B2" s="45"/>
       <c r="C2" s="64" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D2" s="64"/>
       <c r="E2" s="64"/>
@@ -6434,7 +6510,7 @@
         <v>25</v>
       </c>
       <c r="B7" s="49" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C7" s="45"/>
       <c r="D7" s="11">
@@ -6445,7 +6521,7 @@
       </c>
       <c r="F7" s="50"/>
       <c r="G7" s="51" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H7" s="52"/>
       <c r="I7" s="44" t="s">
@@ -6455,7 +6531,9 @@
         <v>9</v>
       </c>
       <c r="K7" s="66"/>
-      <c r="L7" s="46"/>
+      <c r="L7" s="46" t="s">
+        <v>197</v>
+      </c>
       <c r="M7" s="45"/>
     </row>
     <row r="8" spans="1:13" ht="62" customHeight="1" x14ac:dyDescent="0.2">
@@ -6499,7 +6577,7 @@
         <v>31</v>
       </c>
       <c r="B10" s="49" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C10" s="45"/>
       <c r="D10" s="23">
@@ -6510,10 +6588,10 @@
       </c>
       <c r="F10" s="50"/>
       <c r="G10" s="51" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H10" s="53" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I10" s="44" t="s">
         <v>12</v>
@@ -6522,9 +6600,11 @@
         <v>10</v>
       </c>
       <c r="K10" s="63" t="s">
-        <v>182</v>
-      </c>
-      <c r="L10" s="46"/>
+        <v>181</v>
+      </c>
+      <c r="L10" s="46" t="s">
+        <v>196</v>
+      </c>
       <c r="M10" s="56"/>
     </row>
     <row r="11" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -6606,7 +6686,7 @@
         <v>37</v>
       </c>
       <c r="B15" s="49" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C15" s="45"/>
       <c r="D15" s="23">
@@ -6617,7 +6697,7 @@
       </c>
       <c r="F15" s="50"/>
       <c r="G15" s="51" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H15" s="53"/>
       <c r="I15" s="54" t="s">
@@ -6627,7 +6707,9 @@
         <v>9</v>
       </c>
       <c r="K15" s="45"/>
-      <c r="L15" s="58"/>
+      <c r="L15" s="58" t="s">
+        <v>196</v>
+      </c>
       <c r="M15" s="45"/>
     </row>
     <row r="16" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -6709,7 +6791,7 @@
         <v>39</v>
       </c>
       <c r="B20" s="49" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C20" s="45"/>
       <c r="D20" s="23">
@@ -6720,7 +6802,7 @@
       </c>
       <c r="F20" s="50"/>
       <c r="G20" s="51" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H20" s="53"/>
       <c r="I20" s="54" t="s">
@@ -6730,7 +6812,9 @@
         <v>9</v>
       </c>
       <c r="K20" s="45"/>
-      <c r="L20" s="58"/>
+      <c r="L20" s="58" t="s">
+        <v>197</v>
+      </c>
       <c r="M20" s="45"/>
     </row>
     <row r="21" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -6812,7 +6896,7 @@
         <v>43</v>
       </c>
       <c r="B25" s="49" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C25" s="45"/>
       <c r="D25" s="23">
@@ -6823,10 +6907,10 @@
       </c>
       <c r="F25" s="50"/>
       <c r="G25" s="51" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H25" s="53" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I25" s="54" t="s">
         <v>51</v>
@@ -6835,9 +6919,11 @@
         <v>10</v>
       </c>
       <c r="K25" s="63" t="s">
-        <v>176</v>
-      </c>
-      <c r="L25" s="58"/>
+        <v>175</v>
+      </c>
+      <c r="L25" s="58" t="s">
+        <v>197</v>
+      </c>
       <c r="M25" s="45"/>
     </row>
     <row r="26" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -6919,7 +7005,7 @@
         <v>48</v>
       </c>
       <c r="B30" s="49" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C30" s="45"/>
       <c r="D30" s="23">
@@ -6930,10 +7016,10 @@
       </c>
       <c r="F30" s="50"/>
       <c r="G30" s="51" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H30" s="53" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I30" s="54" t="s">
         <v>51</v>
@@ -6942,9 +7028,11 @@
         <v>10</v>
       </c>
       <c r="K30" s="63" t="s">
-        <v>176</v>
-      </c>
-      <c r="L30" s="58"/>
+        <v>175</v>
+      </c>
+      <c r="L30" s="58" t="s">
+        <v>196</v>
+      </c>
       <c r="M30" s="45"/>
     </row>
     <row r="31" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -7026,7 +7114,7 @@
         <v>48</v>
       </c>
       <c r="B35" s="49" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C35" s="45"/>
       <c r="D35" s="23">
@@ -7037,7 +7125,7 @@
       </c>
       <c r="F35" s="50"/>
       <c r="G35" s="51" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H35" s="53"/>
       <c r="I35" s="54" t="s">
@@ -7047,7 +7135,9 @@
         <v>9</v>
       </c>
       <c r="K35" s="45"/>
-      <c r="L35" s="58"/>
+      <c r="L35" s="58" t="s">
+        <v>197</v>
+      </c>
       <c r="M35" s="45"/>
     </row>
     <row r="36" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -7109,7 +7199,7 @@
     </row>
     <row r="39" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="47" t="s">
-        <v>52</v>
+        <v>198</v>
       </c>
       <c r="B39" s="48"/>
       <c r="C39" s="48"/>
@@ -7126,10 +7216,10 @@
     </row>
     <row r="40" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="49" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B40" s="49" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C40" s="45"/>
       <c r="D40" s="23">
@@ -7140,7 +7230,7 @@
       </c>
       <c r="F40" s="50"/>
       <c r="G40" s="51" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H40" s="53"/>
       <c r="I40" s="54" t="s">
@@ -7150,7 +7240,9 @@
         <v>9</v>
       </c>
       <c r="K40" s="45"/>
-      <c r="L40" s="58"/>
+      <c r="L40" s="58" t="s">
+        <v>196</v>
+      </c>
       <c r="M40" s="45"/>
     </row>
     <row r="41" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -7180,7 +7272,7 @@
         <v>3</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F42" s="50"/>
       <c r="G42" s="52"/>
@@ -7212,7 +7304,7 @@
     </row>
     <row r="44" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="47" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B44" s="48"/>
       <c r="C44" s="48"/>
@@ -7229,10 +7321,10 @@
     </row>
     <row r="45" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="49" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B45" s="49" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C45" s="45"/>
       <c r="D45" s="23">
@@ -7243,7 +7335,7 @@
       </c>
       <c r="F45" s="50"/>
       <c r="G45" s="51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H45" s="53"/>
       <c r="I45" s="54" t="s">
@@ -7264,7 +7356,7 @@
         <v>2</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F46" s="50"/>
       <c r="G46" s="52"/>
@@ -7277,7 +7369,7 @@
     </row>
     <row r="47" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="47" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B47" s="48"/>
       <c r="C47" s="48"/>
@@ -7294,10 +7386,10 @@
     </row>
     <row r="48" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="49" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B48" s="49" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C48" s="45"/>
       <c r="D48" s="23">
@@ -7308,7 +7400,7 @@
       </c>
       <c r="F48" s="50"/>
       <c r="G48" s="51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H48" s="53"/>
       <c r="I48" s="44" t="s">
@@ -7318,7 +7410,9 @@
         <v>9</v>
       </c>
       <c r="K48" s="45"/>
-      <c r="L48" s="46"/>
+      <c r="L48" s="46" t="s">
+        <v>197</v>
+      </c>
       <c r="M48" s="45"/>
     </row>
     <row r="49" spans="1:13" ht="32" x14ac:dyDescent="0.2">
@@ -7329,7 +7423,7 @@
         <v>2</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F49" s="50"/>
       <c r="G49" s="52"/>
@@ -7469,157 +7563,183 @@
     <mergeCell ref="H48:H49"/>
   </mergeCells>
   <conditionalFormatting sqref="L4:L5 J5:K5 G2:I3 G5:H5 I5:I18 G50:I1048576 G7:H8 G10:H13">
-    <cfRule type="cellIs" dxfId="152" priority="130" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="136" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J50:L489 J2:L18">
-    <cfRule type="cellIs" dxfId="151" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="80" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="150" priority="131" operator="equal">
+    <cfRule type="cellIs" dxfId="156" priority="137" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="149" priority="132" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="138" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15:H18">
-    <cfRule type="cellIs" dxfId="148" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="57" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G20:G23">
-    <cfRule type="cellIs" dxfId="147" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="50" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I19:I23">
-    <cfRule type="cellIs" dxfId="146" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="54" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J19:L23">
-    <cfRule type="cellIs" dxfId="145" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="53" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="144" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="55" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="143" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="56" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H20:H23">
-    <cfRule type="cellIs" dxfId="142" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="52" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G15:G18">
-    <cfRule type="cellIs" dxfId="141" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="51" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G25:G28">
-    <cfRule type="cellIs" dxfId="140" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="44" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G30:G33">
-    <cfRule type="cellIs" dxfId="139" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="38" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G35:G38">
-    <cfRule type="cellIs" dxfId="138" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="31" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G45:G46">
-    <cfRule type="cellIs" dxfId="137" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="19" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I24:I28">
-    <cfRule type="cellIs" dxfId="136" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="47" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J24:L28">
-    <cfRule type="cellIs" dxfId="135" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="46" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="134" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="48" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="133" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="49" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25:H28">
-    <cfRule type="cellIs" dxfId="132" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="45" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I29:I33">
-    <cfRule type="cellIs" dxfId="131" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="41" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J29:L29 J30:J33 L30:L33">
-    <cfRule type="cellIs" dxfId="130" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="40" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="129" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="42" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="128" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="43" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H30:H33">
-    <cfRule type="cellIs" dxfId="127" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="39" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I34:I38">
-    <cfRule type="cellIs" dxfId="126" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="35" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J34:L38">
-    <cfRule type="cellIs" dxfId="125" priority="28" operator="equal">
+  <conditionalFormatting sqref="J34:L34 J35:K38">
+    <cfRule type="cellIs" dxfId="131" priority="34" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="124" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="36" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="123" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="37" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I39:I43">
-    <cfRule type="cellIs" dxfId="122" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="28" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J39:L43">
-    <cfRule type="cellIs" dxfId="121" priority="21" operator="equal">
+  <conditionalFormatting sqref="J39:L39 J40:K43">
+    <cfRule type="cellIs" dxfId="127" priority="27" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="120" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="29" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="119" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="30" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I44:I46">
+    <cfRule type="cellIs" dxfId="124" priority="22" operator="equal">
+      <formula>"Skipped"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J44:L46">
+    <cfRule type="cellIs" dxfId="123" priority="21" operator="equal">
+      <formula>"Skipped"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="122" priority="23" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="121" priority="24" operator="equal">
+      <formula>"Passed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H45:H46">
+    <cfRule type="cellIs" dxfId="120" priority="20" operator="equal">
+      <formula>"Skipped"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G48:G49">
+    <cfRule type="cellIs" dxfId="119" priority="13" operator="equal">
+      <formula>"Skipped"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I47:I49">
     <cfRule type="cellIs" dxfId="118" priority="16" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J44:L46">
+  <conditionalFormatting sqref="J47:L49">
     <cfRule type="cellIs" dxfId="117" priority="15" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
@@ -7630,60 +7750,56 @@
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H45:H46">
+  <conditionalFormatting sqref="H48:H49">
     <cfRule type="cellIs" dxfId="114" priority="14" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G48:G49">
-    <cfRule type="cellIs" dxfId="113" priority="7" operator="equal">
-      <formula>"Skipped"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I47:I49">
-    <cfRule type="cellIs" dxfId="112" priority="10" operator="equal">
-      <formula>"Skipped"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J47:L49">
-    <cfRule type="cellIs" dxfId="111" priority="9" operator="equal">
-      <formula>"Skipped"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="110" priority="11" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="109" priority="12" operator="equal">
-      <formula>"Passed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H48:H49">
-    <cfRule type="cellIs" dxfId="108" priority="8" operator="equal">
-      <formula>"Skipped"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="H35:H38">
-    <cfRule type="cellIs" dxfId="107" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="12" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H40:H43">
-    <cfRule type="cellIs" dxfId="106" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="11" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G40:G43">
-    <cfRule type="cellIs" dxfId="105" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="10" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30:K33">
-    <cfRule type="cellIs" dxfId="104" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="7" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="103" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="8" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="9" operator="equal">
+      <formula>"Passed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L35:L38">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+      <formula>"Skipped"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+      <formula>"Passed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L40:L43">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"Skipped"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7691,7 +7807,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F50:F1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Passed, Failed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L7:L8 L15:L18 L10:L13 G2:H3 G50:I1048576 L20:L23 L25:L28 L30:L33 L35:L38 L40:L43 L45:L46 L48:L49" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L7:L8 L15:L18 L10:L13 G2:H3 G50:I1048576 L20:L23 L25:L28 L30:L33 L48:L49 L35:L38 L45:L46 L40:L43" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J7:J8 J10:J11 J15:J16 J20:J21 J25:J26 J30:J31 J35:J36 J40:J41 J45:J46 J48:J49" xr:uid="{00000000-0002-0000-0100-000002000000}">
@@ -7760,7 +7876,7 @@
       <c r="A2" s="45"/>
       <c r="B2" s="45"/>
       <c r="C2" s="64" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D2" s="64"/>
       <c r="E2" s="64"/>
@@ -7879,7 +7995,7 @@
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="47" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B6" s="48"/>
       <c r="C6" s="48"/>
@@ -7896,21 +8012,21 @@
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="49" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" s="49" t="s">
         <v>108</v>
-      </c>
-      <c r="B7" s="49" t="s">
-        <v>109</v>
       </c>
       <c r="C7" s="45"/>
       <c r="D7" s="23">
         <v>1</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F7" s="50"/>
       <c r="G7" s="51" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H7" s="52"/>
       <c r="I7" s="44" t="s">
@@ -7944,7 +8060,7 @@
     </row>
     <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="47" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B9" s="48"/>
       <c r="C9" s="48"/>
@@ -7961,21 +8077,21 @@
     </row>
     <row r="10" spans="1:13" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="49" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B10" s="49" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C10" s="45"/>
       <c r="D10" s="31">
         <v>1</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F10" s="50"/>
       <c r="G10" s="51" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H10" s="52"/>
       <c r="I10" s="44" t="s">
@@ -7996,7 +8112,7 @@
         <v>2</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F11" s="50"/>
       <c r="G11" s="52"/>
@@ -8009,7 +8125,7 @@
     </row>
     <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="47" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B12" s="48"/>
       <c r="C12" s="48"/>
@@ -8026,24 +8142,24 @@
     </row>
     <row r="13" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="49" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B13" s="49" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C13" s="45"/>
       <c r="D13" s="31">
         <v>1</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F13" s="50"/>
       <c r="G13" s="51" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H13" s="52" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I13" s="44" t="s">
         <v>12</v>
@@ -8063,7 +8179,7 @@
         <v>2</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F14" s="50"/>
       <c r="G14" s="52"/>
@@ -8076,7 +8192,7 @@
     </row>
     <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="47" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B15" s="48"/>
       <c r="C15" s="48"/>
@@ -8093,24 +8209,24 @@
     </row>
     <row r="16" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="49" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B16" s="49" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C16" s="45"/>
       <c r="D16" s="31">
         <v>1</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F16" s="50"/>
       <c r="G16" s="51" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H16" s="52" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I16" s="44" t="s">
         <v>12</v>
@@ -8130,7 +8246,7 @@
         <v>2</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F17" s="50"/>
       <c r="G17" s="52"/>
@@ -8143,7 +8259,7 @@
     </row>
     <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="47" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B18" s="48"/>
       <c r="C18" s="48"/>
@@ -8160,24 +8276,24 @@
     </row>
     <row r="19" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="49" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B19" s="49" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C19" s="45"/>
       <c r="D19" s="31">
         <v>1</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F19" s="50"/>
       <c r="G19" s="51" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H19" s="52" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I19" s="44" t="s">
         <v>12</v>
@@ -8197,7 +8313,7 @@
         <v>2</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F20" s="50"/>
       <c r="G20" s="52"/>
@@ -8210,7 +8326,7 @@
     </row>
     <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="47" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B21" s="48"/>
       <c r="C21" s="48"/>
@@ -8227,21 +8343,21 @@
     </row>
     <row r="22" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="49" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B22" s="49" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C22" s="45"/>
       <c r="D22" s="31">
         <v>1</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F22" s="50"/>
       <c r="G22" s="51" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H22" s="52"/>
       <c r="I22" s="44" t="s">
@@ -8262,7 +8378,7 @@
         <v>2</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F23" s="50"/>
       <c r="G23" s="52"/>
@@ -8354,113 +8470,113 @@
     <mergeCell ref="C10:C11"/>
   </mergeCells>
   <conditionalFormatting sqref="L4:L5 J5:K5 G2:I3 G5:H5 I5:I8 G24:I1048576 G7:H8">
-    <cfRule type="cellIs" dxfId="101" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="47" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J24:L463 J2:L8">
-    <cfRule type="cellIs" dxfId="100" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="46" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="99" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="48" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="49" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9:I11 G10:H11">
-    <cfRule type="cellIs" dxfId="97" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="21" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:L11">
-    <cfRule type="cellIs" dxfId="96" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="20" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="95" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="22" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="23" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12:I14 G13:H14">
-    <cfRule type="cellIs" dxfId="93" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="17" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12:L14">
-    <cfRule type="cellIs" dxfId="92" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="16" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="91" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="18" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="19" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I15:I17 G16:G17">
-    <cfRule type="cellIs" dxfId="89" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="13" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15:L17">
-    <cfRule type="cellIs" dxfId="88" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="12" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="14" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="15" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I18:I20 G19:G20">
-    <cfRule type="cellIs" dxfId="85" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="9" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J18:L20">
-    <cfRule type="cellIs" dxfId="84" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="8" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="10" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="11" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16:H17">
-    <cfRule type="cellIs" dxfId="81" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="7" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H19:H20">
-    <cfRule type="cellIs" dxfId="80" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="6" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I21:I23 G22:G23">
-    <cfRule type="cellIs" dxfId="79" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="3" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J21:L23">
-    <cfRule type="cellIs" dxfId="78" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="2" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="4" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="5" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22:H23">
-    <cfRule type="cellIs" dxfId="75" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="1" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8515,7 +8631,7 @@
       <c r="A1" s="45"/>
       <c r="B1" s="45"/>
       <c r="C1" s="65" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D1" s="65"/>
       <c r="E1" s="65"/>
@@ -8532,7 +8648,7 @@
       <c r="A2" s="45"/>
       <c r="B2" s="45"/>
       <c r="C2" s="64" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D2" s="64"/>
       <c r="E2" s="64"/>
@@ -8668,26 +8784,26 @@
     </row>
     <row r="7" spans="1:13" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B7" s="27" t="s">
         <v>36</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D7" s="23">
         <v>1</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F7" s="30"/>
       <c r="G7" s="28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H7" s="29" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I7" s="25" t="s">
         <v>12</v>
@@ -8696,14 +8812,14 @@
         <v>10</v>
       </c>
       <c r="K7" s="40" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L7" s="26"/>
       <c r="M7" s="24"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="47" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B8" s="48"/>
       <c r="C8" s="48"/>
@@ -8720,7 +8836,7 @@
     </row>
     <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="49" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B9" s="49" t="s">
         <v>36</v>
@@ -8730,14 +8846,14 @@
         <v>1</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F9" s="50"/>
       <c r="G9" s="51" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H9" s="53" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I9" s="44" t="s">
         <v>12</v>
@@ -8746,7 +8862,7 @@
         <v>10</v>
       </c>
       <c r="K9" s="63" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="L9" s="46"/>
       <c r="M9" s="45"/>
@@ -8759,7 +8875,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F10" s="50"/>
       <c r="G10" s="52"/>
@@ -8772,7 +8888,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="47" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B11" s="48"/>
       <c r="C11" s="48"/>
@@ -8789,13 +8905,13 @@
     </row>
     <row r="12" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="49" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B12" s="49" t="s">
         <v>36</v>
       </c>
       <c r="C12" s="45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D12" s="31">
         <v>1</v>
@@ -8805,7 +8921,7 @@
       </c>
       <c r="F12" s="50"/>
       <c r="G12" s="51" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H12" s="53"/>
       <c r="I12" s="44" t="s">
@@ -8839,7 +8955,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="47" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B14" s="48"/>
       <c r="C14" s="48"/>
@@ -8856,13 +8972,13 @@
     </row>
     <row r="15" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="49" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B15" s="49" t="s">
         <v>36</v>
       </c>
       <c r="C15" s="45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D15" s="31">
         <v>1</v>
@@ -8872,7 +8988,7 @@
       </c>
       <c r="F15" s="50"/>
       <c r="G15" s="51" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H15" s="53"/>
       <c r="I15" s="44" t="s">
@@ -8906,7 +9022,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="47" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B17" s="48"/>
       <c r="C17" s="48"/>
@@ -8923,13 +9039,13 @@
     </row>
     <row r="18" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="49" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B18" s="49" t="s">
         <v>36</v>
       </c>
       <c r="C18" s="45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D18" s="31">
         <v>1</v>
@@ -8939,7 +9055,7 @@
       </c>
       <c r="F18" s="50"/>
       <c r="G18" s="51" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H18" s="53"/>
       <c r="I18" s="44" t="s">
@@ -8973,7 +9089,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="47" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B20" s="48"/>
       <c r="C20" s="48"/>
@@ -8990,23 +9106,23 @@
     </row>
     <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="49" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B21" s="49" t="s">
         <v>36</v>
       </c>
       <c r="C21" s="45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D21" s="31">
         <v>1</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F21" s="50"/>
       <c r="G21" s="51" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H21" s="53"/>
       <c r="I21" s="44" t="s">
@@ -9040,7 +9156,7 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="47" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B23" s="48"/>
       <c r="C23" s="48"/>
@@ -9057,13 +9173,13 @@
     </row>
     <row r="24" spans="1:13" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="49" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B24" s="49" t="s">
         <v>36</v>
       </c>
       <c r="C24" s="45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D24" s="31">
         <v>1</v>
@@ -9073,7 +9189,7 @@
       </c>
       <c r="F24" s="50"/>
       <c r="G24" s="51" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H24" s="53"/>
       <c r="I24" s="44" t="s">
@@ -9107,7 +9223,7 @@
     </row>
     <row r="26" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="47" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B26" s="48"/>
       <c r="C26" s="48"/>
@@ -9124,13 +9240,13 @@
     </row>
     <row r="27" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="49" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B27" s="49" t="s">
         <v>36</v>
       </c>
       <c r="C27" s="45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D27" s="31">
         <v>1</v>
@@ -9140,7 +9256,7 @@
       </c>
       <c r="F27" s="50"/>
       <c r="G27" s="51" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H27" s="53"/>
       <c r="I27" s="54" t="s">
@@ -9180,7 +9296,7 @@
         <v>3</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F29" s="50"/>
       <c r="G29" s="52"/>
@@ -9193,7 +9309,7 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="47" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B30" s="48"/>
       <c r="C30" s="48"/>
@@ -9210,13 +9326,13 @@
     </row>
     <row r="31" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="49" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B31" s="49" t="s">
         <v>36</v>
       </c>
       <c r="C31" s="45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D31" s="31">
         <v>1</v>
@@ -9226,7 +9342,7 @@
       </c>
       <c r="F31" s="50"/>
       <c r="G31" s="51" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H31" s="53"/>
       <c r="I31" s="44" t="s">
@@ -9260,7 +9376,7 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="47" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B33" s="48"/>
       <c r="C33" s="48"/>
@@ -9277,13 +9393,13 @@
     </row>
     <row r="34" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="67" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B34" s="67" t="s">
         <v>36</v>
       </c>
       <c r="C34" s="56" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D34" s="31">
         <v>1</v>
@@ -9293,7 +9409,7 @@
       </c>
       <c r="F34" s="70"/>
       <c r="G34" s="73" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H34" s="76"/>
       <c r="I34" s="54" t="s">
@@ -9333,7 +9449,7 @@
         <v>3</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F36" s="72"/>
       <c r="G36" s="75"/>
@@ -9346,7 +9462,7 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="47" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B37" s="48"/>
       <c r="C37" s="48"/>
@@ -9363,13 +9479,13 @@
     </row>
     <row r="38" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="67" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B38" s="67" t="s">
         <v>36</v>
       </c>
       <c r="C38" s="56" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D38" s="31">
         <v>1</v>
@@ -9379,7 +9495,7 @@
       </c>
       <c r="F38" s="70"/>
       <c r="G38" s="73" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H38" s="76"/>
       <c r="I38" s="54" t="s">
@@ -9419,7 +9535,7 @@
         <v>3</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F40" s="71"/>
       <c r="G40" s="74"/>
@@ -9432,7 +9548,7 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="47" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B41" s="48"/>
       <c r="C41" s="48"/>
@@ -9449,13 +9565,13 @@
     </row>
     <row r="42" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="67" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B42" s="67" t="s">
         <v>36</v>
       </c>
       <c r="C42" s="56" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D42" s="31">
         <v>1</v>
@@ -9465,7 +9581,7 @@
       </c>
       <c r="F42" s="70"/>
       <c r="G42" s="73" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H42" s="76"/>
       <c r="I42" s="54" t="s">
@@ -9505,7 +9621,7 @@
         <v>3</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F44" s="71"/>
       <c r="G44" s="74"/>
@@ -9518,7 +9634,7 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" s="47" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B45" s="48"/>
       <c r="C45" s="48"/>
@@ -9535,13 +9651,13 @@
     </row>
     <row r="46" spans="1:13" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="49" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B46" s="49" t="s">
         <v>36</v>
       </c>
       <c r="C46" s="45" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D46" s="31">
         <v>1</v>
@@ -9551,7 +9667,7 @@
       </c>
       <c r="F46" s="50"/>
       <c r="G46" s="51" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H46" s="53"/>
       <c r="I46" s="44" t="s">
@@ -9585,7 +9701,7 @@
     </row>
     <row r="48" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="47" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B48" s="48"/>
       <c r="C48" s="48"/>
@@ -9602,13 +9718,13 @@
     </row>
     <row r="49" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="49" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B49" s="49" t="s">
         <v>36</v>
       </c>
       <c r="C49" s="45" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D49" s="31">
         <v>1</v>
@@ -9618,7 +9734,7 @@
       </c>
       <c r="F49" s="50"/>
       <c r="G49" s="51" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H49" s="53"/>
       <c r="I49" s="54" t="s">
@@ -9652,7 +9768,7 @@
     </row>
     <row r="51" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="47" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B51" s="48"/>
       <c r="C51" s="48"/>
@@ -9669,13 +9785,13 @@
     </row>
     <row r="52" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="49" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B52" s="49" t="s">
         <v>36</v>
       </c>
       <c r="C52" s="45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D52" s="31">
         <v>1</v>
@@ -9685,7 +9801,7 @@
       </c>
       <c r="F52" s="50"/>
       <c r="G52" s="51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H52" s="53"/>
       <c r="I52" s="54" t="s">
@@ -9706,7 +9822,7 @@
         <v>2</v>
       </c>
       <c r="E53" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F53" s="50"/>
       <c r="G53" s="52"/>
@@ -9719,7 +9835,7 @@
     </row>
     <row r="54" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="47" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B54" s="48"/>
       <c r="C54" s="48"/>
@@ -9736,13 +9852,13 @@
     </row>
     <row r="55" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="49" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B55" s="49" t="s">
         <v>36</v>
       </c>
       <c r="C55" s="45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D55" s="31">
         <v>1</v>
@@ -9752,7 +9868,7 @@
       </c>
       <c r="F55" s="50"/>
       <c r="G55" s="51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H55" s="53"/>
       <c r="I55" s="44" t="s">
@@ -9773,7 +9889,7 @@
         <v>2</v>
       </c>
       <c r="E56" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F56" s="50"/>
       <c r="G56" s="52"/>
@@ -9973,317 +10089,317 @@
     <mergeCell ref="B9:B10"/>
   </mergeCells>
   <conditionalFormatting sqref="J2:L5 J57:L355">
-    <cfRule type="cellIs" dxfId="74" priority="402" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="402" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="403" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="403" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="404" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="404" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4 G2:I3 I30:I32 G31:H32 G26:I29 I45:I50">
-    <cfRule type="cellIs" dxfId="71" priority="394" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="394" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:L4">
-    <cfRule type="cellIs" dxfId="70" priority="353" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="353" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J26:L32 J45:L50">
-    <cfRule type="cellIs" dxfId="69" priority="345" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="345" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="346" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="346" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="347" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="347" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:I10 G7:H10">
-    <cfRule type="cellIs" dxfId="66" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="80" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:L10">
-    <cfRule type="cellIs" dxfId="65" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="79" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="81" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="82" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8:I10 G9:H10">
-    <cfRule type="cellIs" dxfId="62" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="76" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:L10">
-    <cfRule type="cellIs" dxfId="61" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="75" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="77" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="78" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G18:G19">
-    <cfRule type="cellIs" dxfId="58" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="54" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J20:L22">
-    <cfRule type="cellIs" dxfId="57" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="49" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="51" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="52" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11:I13 H12:H13">
-    <cfRule type="cellIs" dxfId="54" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="68" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11:L13">
-    <cfRule type="cellIs" dxfId="53" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="67" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="69" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="70" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12:G13">
-    <cfRule type="cellIs" dxfId="50" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="66" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12:G13">
-    <cfRule type="cellIs" dxfId="49" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="65" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14:I16 H15:H16">
-    <cfRule type="cellIs" dxfId="48" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="62" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J14:L16">
-    <cfRule type="cellIs" dxfId="47" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="61" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="63" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="64" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G15:G16">
-    <cfRule type="cellIs" dxfId="44" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="60" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G15:G16">
-    <cfRule type="cellIs" dxfId="43" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="59" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I17:I19 H18:H19">
-    <cfRule type="cellIs" dxfId="42" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="56" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J17:L19">
-    <cfRule type="cellIs" dxfId="41" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="55" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="57" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="58" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20:I22 G21:H22">
-    <cfRule type="cellIs" dxfId="38" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="50" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G18:G19">
-    <cfRule type="cellIs" dxfId="37" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="53" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I23:I29 G24:H29">
-    <cfRule type="cellIs" dxfId="36" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="46" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J23:L29">
-    <cfRule type="cellIs" dxfId="35" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="45" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="47" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="48" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I33:I34 G34:H34">
-    <cfRule type="cellIs" dxfId="32" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="38" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J33:L34">
-    <cfRule type="cellIs" dxfId="31" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="37" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="39" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="40" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I37:I38 G38:H38">
-    <cfRule type="cellIs" dxfId="28" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="34" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J37:L38">
-    <cfRule type="cellIs" dxfId="27" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="33" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="35" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="36" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I41:I42 G42:H42">
-    <cfRule type="cellIs" dxfId="24" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="30" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J41:L42">
-    <cfRule type="cellIs" dxfId="23" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="29" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="31" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="32" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G52:G53">
-    <cfRule type="cellIs" dxfId="20" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="23" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I51:I53">
-    <cfRule type="cellIs" dxfId="19" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="26" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J51:L53">
-    <cfRule type="cellIs" dxfId="18" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="25" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="27" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="28" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H52:H53">
-    <cfRule type="cellIs" dxfId="15" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="24" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G55:G56">
-    <cfRule type="cellIs" dxfId="14" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="17" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I54:I56">
-    <cfRule type="cellIs" dxfId="13" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="20" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J54:L56">
-    <cfRule type="cellIs" dxfId="12" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="19" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="21" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="22" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H55:H56">
-    <cfRule type="cellIs" dxfId="9" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="18" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G27:G29">
-    <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="11" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I26:I29">
-    <cfRule type="cellIs" dxfId="7" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J26:L29">
-    <cfRule type="cellIs" dxfId="6" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="16" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27:H29">
-    <cfRule type="cellIs" dxfId="3" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G46:H47">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H49:H50">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G49:G50">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10316,7 +10432,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F06CBE9-20CC-0441-8560-ECE826D51085}">
   <dimension ref="A1:Y16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -11286,7 +11402,7 @@
   <sheetData>
     <row r="1" spans="1:24" ht="20" x14ac:dyDescent="0.2">
       <c r="A1" s="80" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B1" s="80"/>
       <c r="C1" s="80"/>
@@ -11305,28 +11421,28 @@
     </row>
     <row r="3" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="81" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B3" s="81"/>
       <c r="C3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="81" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B4" s="81"/>
     </row>
     <row r="5" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="81" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B5" s="81"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" s="82" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B7" s="83"/>
       <c r="C7" s="83"/>
@@ -11345,7 +11461,7 @@
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" s="79" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B8" s="79"/>
       <c r="C8" s="79"/>
@@ -11364,52 +11480,52 @@
     </row>
     <row r="10" spans="1:24" ht="42" x14ac:dyDescent="0.2">
       <c r="A10" s="35" t="s">
+        <v>149</v>
+      </c>
+      <c r="B10" s="35" t="s">
         <v>150</v>
       </c>
-      <c r="B10" s="35" t="s">
+      <c r="C10" s="35" t="s">
         <v>151</v>
       </c>
-      <c r="C10" s="35" t="s">
+      <c r="D10" s="35" t="s">
         <v>152</v>
       </c>
-      <c r="D10" s="35" t="s">
+      <c r="E10" s="35" t="s">
         <v>153</v>
       </c>
-      <c r="E10" s="35" t="s">
+      <c r="F10" s="35" t="s">
         <v>154</v>
-      </c>
-      <c r="F10" s="35" t="s">
-        <v>155</v>
       </c>
       <c r="G10" s="35" t="s">
         <v>11</v>
       </c>
       <c r="H10" s="35" t="s">
+        <v>155</v>
+      </c>
+      <c r="I10" s="35" t="s">
         <v>156</v>
       </c>
-      <c r="I10" s="35" t="s">
+      <c r="J10" s="35" t="s">
         <v>157</v>
-      </c>
-      <c r="J10" s="35" t="s">
-        <v>158</v>
       </c>
       <c r="K10" s="35" t="s">
         <v>6</v>
       </c>
       <c r="L10" s="35" t="s">
+        <v>158</v>
+      </c>
+      <c r="M10" s="35" t="s">
         <v>159</v>
       </c>
-      <c r="M10" s="35" t="s">
+      <c r="N10" s="35" t="s">
         <v>160</v>
       </c>
-      <c r="N10" s="35" t="s">
+      <c r="O10" s="35" t="s">
         <v>161</v>
       </c>
-      <c r="O10" s="35" t="s">
-        <v>162</v>
-      </c>
       <c r="P10" s="35" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="T10" t="s">
         <v>6</v>
@@ -11418,39 +11534,39 @@
         <v>11</v>
       </c>
       <c r="W10" t="s">
+        <v>162</v>
+      </c>
+      <c r="X10" t="s">
         <v>163</v>
-      </c>
-      <c r="X10" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:24" ht="112" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B11" s="37">
         <v>44266</v>
       </c>
       <c r="C11" s="38" t="s">
+        <v>165</v>
+      </c>
+      <c r="D11" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="E11" s="39" t="s">
         <v>166</v>
       </c>
-      <c r="D11" s="39" t="s">
-        <v>142</v>
-      </c>
-      <c r="E11" s="39" t="s">
+      <c r="F11" s="39" t="s">
         <v>167</v>
       </c>
-      <c r="F11" s="39" t="s">
+      <c r="G11" s="41" t="s">
         <v>168</v>
-      </c>
-      <c r="G11" s="41" t="s">
-        <v>169</v>
       </c>
       <c r="H11" s="41"/>
       <c r="I11" s="42"/>
       <c r="J11" s="41"/>
       <c r="K11" s="41" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L11" s="41"/>
       <c r="M11" s="42"/>
@@ -11458,27 +11574,27 @@
       <c r="O11" s="41"/>
       <c r="P11" s="38"/>
       <c r="T11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="12" spans="1:24" ht="196" x14ac:dyDescent="0.2">
       <c r="A12" s="36" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B12" s="37">
         <v>44266</v>
       </c>
       <c r="C12" s="38" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D12" s="39" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E12" s="39" t="s">
+        <v>171</v>
+      </c>
+      <c r="F12" s="39" t="s">
         <v>172</v>
-      </c>
-      <c r="F12" s="39" t="s">
-        <v>173</v>
       </c>
       <c r="G12" s="43" t="s">
         <v>51</v>
@@ -11487,7 +11603,7 @@
       <c r="I12" s="42"/>
       <c r="J12" s="41"/>
       <c r="K12" s="41" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L12" s="41"/>
       <c r="M12" s="42"/>
@@ -11495,36 +11611,36 @@
       <c r="O12" s="41"/>
       <c r="P12" s="38"/>
       <c r="T12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="V12" t="s">
         <v>12</v>
       </c>
       <c r="W12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="X12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="13" spans="1:24" ht="182" x14ac:dyDescent="0.2">
       <c r="A13" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B13" s="37">
         <v>44266</v>
       </c>
       <c r="C13" s="38" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D13" s="39" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E13" s="39" t="s">
+        <v>176</v>
+      </c>
+      <c r="F13" s="39" t="s">
         <v>177</v>
-      </c>
-      <c r="F13" s="39" t="s">
-        <v>178</v>
       </c>
       <c r="G13" s="43" t="s">
         <v>51</v>
@@ -11533,7 +11649,7 @@
       <c r="I13" s="42"/>
       <c r="J13" s="41"/>
       <c r="K13" s="41" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L13" s="41"/>
       <c r="M13" s="42"/>
@@ -11541,36 +11657,36 @@
       <c r="O13" s="41"/>
       <c r="P13" s="38"/>
       <c r="T13" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="V13" t="s">
         <v>51</v>
       </c>
       <c r="W13" t="s">
+        <v>179</v>
+      </c>
+      <c r="X13" t="s">
         <v>180</v>
-      </c>
-      <c r="X13" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="14" spans="1:24" ht="210" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B14" s="37">
         <v>44266</v>
       </c>
       <c r="C14" s="38" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D14" s="39" t="s">
         <v>36</v>
       </c>
       <c r="E14" s="39" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F14" s="39" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G14" s="43" t="s">
         <v>51</v>
@@ -11579,7 +11695,7 @@
       <c r="I14" s="42"/>
       <c r="J14" s="41"/>
       <c r="K14" s="41" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L14" s="41"/>
       <c r="M14" s="42"/>
@@ -11587,116 +11703,116 @@
       <c r="O14" s="41"/>
       <c r="P14" s="38"/>
       <c r="T14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="V14" t="s">
         <v>51</v>
       </c>
       <c r="W14" t="s">
+        <v>179</v>
+      </c>
+      <c r="X14" t="s">
         <v>180</v>
-      </c>
-      <c r="X14" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="15" spans="1:24" ht="224" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B15" s="37">
         <v>44266</v>
       </c>
       <c r="C15" s="38" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D15" s="39" t="s">
         <v>36</v>
       </c>
       <c r="E15" s="39" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F15" s="39" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G15" s="43" t="s">
         <v>51</v>
       </c>
       <c r="H15" s="41"/>
       <c r="I15" s="42" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J15" s="41"/>
       <c r="K15" s="41" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L15" s="41" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="M15" s="42"/>
       <c r="N15" s="41"/>
       <c r="O15" s="41"/>
       <c r="P15" s="38"/>
       <c r="T15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="V15" t="s">
         <v>51</v>
       </c>
       <c r="W15" t="s">
+        <v>179</v>
+      </c>
+      <c r="X15" t="s">
         <v>180</v>
-      </c>
-      <c r="X15" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="16" spans="1:24" ht="182" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B16" s="37">
         <v>44266</v>
       </c>
       <c r="C16" s="38" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D16" s="39" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E16" s="39" t="s">
+        <v>192</v>
+      </c>
+      <c r="F16" s="39" t="s">
         <v>193</v>
-      </c>
-      <c r="F16" s="39" t="s">
-        <v>194</v>
       </c>
       <c r="G16" s="43" t="s">
         <v>12</v>
       </c>
       <c r="H16" s="41"/>
       <c r="I16" s="42" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J16" s="41"/>
       <c r="K16" s="41" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L16" s="41" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="M16" s="42"/>
       <c r="N16" s="41"/>
       <c r="O16" s="41"/>
       <c r="P16" s="38"/>
       <c r="T16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="V16" t="s">
         <v>51</v>
       </c>
       <c r="W16" t="s">
+        <v>179</v>
+      </c>
+      <c r="X16" t="s">
         <v>180</v>
-      </c>
-      <c r="X16" t="s">
-        <v>181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>